<commit_message>
removed scaffold counting, parallelized adding unmapped sites
</commit_message>
<xml_diff>
--- a/data/referee-performance-owlmonkey.xlsx
+++ b/data/referee-performance-owlmonkey.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bin\referee\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregg/bin/referee/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D678A0ED-E3DF-B748-BB4A-AEC822BAB910}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38280" yWindow="456" windowWidth="28620" windowHeight="12924"/>
+    <workbookView xWindow="-38280" yWindow="460" windowWidth="35660" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="owl-monkey-info" sheetId="4" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="47">
   <si>
     <t>Num procs</t>
   </si>
@@ -154,12 +155,21 @@
   </si>
   <si>
     <t>561.67 GB</t>
+  </si>
+  <si>
+    <t>54 minutes 23 seconds</t>
+  </si>
+  <si>
+    <t>69 GB</t>
+  </si>
+  <si>
+    <t>split by scaffold</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -284,6 +294,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -319,6 +346,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -494,21 +538,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -516,7 +560,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -524,7 +568,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -532,7 +576,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -540,7 +584,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -548,17 +592,26 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -566,7 +619,7 @@
         <v>28921</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -574,67 +627,67 @@
         <v>2861668348</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -645,24 +698,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -682,7 +735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -690,7 +743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -698,7 +751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -706,7 +759,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -714,7 +767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -722,7 +775,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -730,7 +783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -738,7 +791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -746,7 +799,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -754,7 +807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -762,7 +815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -770,7 +823,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -778,7 +831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -786,7 +839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -794,7 +847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -802,7 +855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -810,7 +863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -818,7 +871,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -826,7 +879,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -834,7 +887,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -842,7 +895,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -850,7 +903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -858,7 +911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -866,7 +919,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -874,7 +927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
@@ -882,7 +935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -890,7 +943,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -898,7 +951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -906,7 +959,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -914,7 +967,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -922,7 +975,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -930,7 +983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -938,7 +991,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>5</v>
       </c>
@@ -946,7 +999,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>5</v>
       </c>
@@ -954,7 +1007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>5</v>
       </c>
@@ -962,7 +1015,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>5</v>
       </c>
@@ -970,7 +1023,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>5</v>
       </c>
@@ -978,7 +1031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>5</v>
       </c>
@@ -986,7 +1039,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>5</v>
       </c>
@@ -994,7 +1047,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>5</v>
       </c>
@@ -1002,7 +1055,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>5</v>
       </c>
@@ -1010,7 +1063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>5</v>
       </c>
@@ -1018,7 +1071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>5</v>
       </c>
@@ -1033,24 +1086,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +1123,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1090,7 +1143,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1110,7 +1163,7 @@
         <v>257.2734375</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1130,7 +1183,7 @@
         <v>257.2734375</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1150,7 +1203,7 @@
         <v>257.2734375</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1170,7 +1223,7 @@
         <v>257.2734375</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1190,7 +1243,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1210,7 +1263,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1230,7 +1283,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1250,7 +1303,7 @@
         <v>1176.6484375</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1270,7 +1323,7 @@
         <v>1176.6171875</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1290,7 +1343,7 @@
         <v>1176.6171875</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1310,7 +1363,7 @@
         <v>1176.6171875</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1330,7 +1383,7 @@
         <v>1176.6171875</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1350,7 +1403,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1370,7 +1423,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1390,7 +1443,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1410,7 +1463,7 @@
         <v>1531.890625</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1430,7 +1483,7 @@
         <v>1531.875</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1450,7 +1503,7 @@
         <v>1531.859375</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1470,7 +1523,7 @@
         <v>1531.859375</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1490,7 +1543,7 @@
         <v>1531.859375</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1510,7 +1563,7 @@
         <v>1531.859375</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -1530,7 +1583,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -1550,7 +1603,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1570,7 +1623,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -1590,7 +1643,7 @@
         <v>1887.125</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1610,7 +1663,7 @@
         <v>1887.125</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -1630,7 +1683,7 @@
         <v>1887.109375</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1650,7 +1703,7 @@
         <v>1887.09375</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -1670,7 +1723,7 @@
         <v>1887.09375</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1690,7 +1743,7 @@
         <v>1887.09375</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -1710,7 +1763,7 @@
         <v>1887.09375</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>5</v>
       </c>
@@ -1730,7 +1783,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>5</v>
       </c>
@@ -1750,7 +1803,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>5</v>
       </c>
@@ -1770,7 +1823,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>5</v>
       </c>
@@ -1790,7 +1843,7 @@
         <v>2242.3515625</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>5</v>
       </c>
@@ -1810,7 +1863,7 @@
         <v>2242.3515625</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>5</v>
       </c>
@@ -1830,7 +1883,7 @@
         <v>2242.3515625</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>5</v>
       </c>
@@ -1850,7 +1903,7 @@
         <v>2242.3359375</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>5</v>
       </c>
@@ -1870,7 +1923,7 @@
         <v>2242.3359375</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>5</v>
       </c>
@@ -1890,7 +1943,7 @@
         <v>2242.3359375</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>5</v>
       </c>
@@ -1910,7 +1963,7 @@
         <v>2242.3359375</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>5</v>
       </c>
@@ -1936,24 +1989,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1973,7 +2026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1981,7 +2034,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1989,7 +2042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1997,7 +2050,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2005,7 +2058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2013,7 +2066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2021,7 +2074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2029,7 +2082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2037,7 +2090,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2045,7 +2098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2053,7 +2106,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2061,7 +2114,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2069,7 +2122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2077,7 +2130,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2085,7 +2138,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2093,7 +2146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2101,7 +2154,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2109,7 +2162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2117,7 +2170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2125,7 +2178,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2133,7 +2186,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2141,7 +2194,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2149,7 +2202,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -2157,7 +2210,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -2165,7 +2218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
@@ -2173,7 +2226,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2181,7 +2234,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2189,7 +2242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2197,7 +2250,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2205,7 +2258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2213,7 +2266,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2221,7 +2274,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2229,7 +2282,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>5</v>
       </c>
@@ -2237,7 +2290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>5</v>
       </c>
@@ -2245,7 +2298,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>5</v>
       </c>
@@ -2253,7 +2306,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>5</v>
       </c>
@@ -2261,7 +2314,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>5</v>
       </c>
@@ -2269,7 +2322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>5</v>
       </c>
@@ -2277,7 +2330,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>5</v>
       </c>
@@ -2285,7 +2338,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>5</v>
       </c>
@@ -2293,7 +2346,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>5</v>
       </c>
@@ -2301,7 +2354,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>5</v>
       </c>
@@ -2309,7 +2362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
added perf page (unlinked)
</commit_message>
<xml_diff>
--- a/data/referee-performance-owlmonkey.xlsx
+++ b/data/referee-performance-owlmonkey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregg/bin/referee/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1B3EB3-9BE1-8D4C-879F-37CA432BE6E0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF6ABF8-7152-D04A-9073-2061EF730AE8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37200" yWindow="460" windowWidth="35660" windowHeight="16320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="35660" windowHeight="16320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="owl-monkey-info" sheetId="4" r:id="rId1"/>
@@ -736,7 +736,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -776,6 +776,18 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2">
+        <v>90.856513023399998</v>
+      </c>
+      <c r="D2">
+        <v>90.872089862799996</v>
+      </c>
+      <c r="E2">
+        <v>38.98828125</v>
+      </c>
+      <c r="F2">
+        <v>168.953125</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -784,6 +796,18 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3">
+        <v>18.001127004600001</v>
+      </c>
+      <c r="D3">
+        <v>108.873216867</v>
+      </c>
+      <c r="E3">
+        <v>49.51171875</v>
+      </c>
+      <c r="F3">
+        <v>179.46875</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -792,6 +816,18 @@
       <c r="B4" t="s">
         <v>50</v>
       </c>
+      <c r="C4">
+        <v>1.36613845825E-3</v>
+      </c>
+      <c r="D4">
+        <v>49258.458025</v>
+      </c>
+      <c r="E4">
+        <v>102.07421875</v>
+      </c>
+      <c r="F4">
+        <v>233.19921875</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -799,6 +835,18 @@
       </c>
       <c r="B5" t="s">
         <v>10</v>
+      </c>
+      <c r="C5">
+        <v>3.7100315094E-3</v>
+      </c>
+      <c r="D5">
+        <v>62391.398842800001</v>
+      </c>
+      <c r="E5">
+        <v>102.125</v>
+      </c>
+      <c r="F5">
+        <v>233.15234375</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>